<commit_message>
Attempt VI - Rectified pilates config file for duplicated beam.warmStart.type parameter. Correctly it should be set to beam.warmStart.type = "linkStatsFromLastRun"
</commit_message>
<xml_diff>
--- a/SpeedCalculations.xlsx
+++ b/SpeedCalculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LBNL\LBNL-BEAM\beam-data-austin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF0C3FE-42C9-4917-87FF-8979350BA798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E082A44-593F-4837-89C4-61F3893E60AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9435" yWindow="780" windowWidth="13605" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27240" yWindow="1200" windowWidth="13605" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>motorway</t>
   </si>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,17 +420,24 @@
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1">
         <v>45070</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1">
+        <v>0.08</v>
+      </c>
+      <c r="F1">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -443,8 +450,14 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -458,8 +471,16 @@
         <f>B3*C3</f>
         <v>26.285951999999998</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f>56.5051/67.3424</f>
+        <v>0.83907166955736656</v>
+      </c>
+      <c r="F3">
+        <f>56.5051/67.3424</f>
+        <v>0.83907166955736656</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -473,8 +494,16 @@
         <f t="shared" ref="D4:D15" si="0">B4*C4</f>
         <v>23.246080000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f>51.6663/64.7336</f>
+        <v>0.79813728882682256</v>
+      </c>
+      <c r="F4">
+        <f>51.6663/64.7336</f>
+        <v>0.79813728882682256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -488,8 +517,16 @@
         <f t="shared" si="0"/>
         <v>19.216799999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f>42.9408/47.1749</f>
+        <v>0.91024676257925297</v>
+      </c>
+      <c r="F5">
+        <f>42.9408/47.1749</f>
+        <v>0.91024676257925297</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -503,8 +540,16 @@
         <f t="shared" si="0"/>
         <v>14.29344</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f>31.7833/35.5311</f>
+        <v>0.89452057493294601</v>
+      </c>
+      <c r="F6">
+        <f>31.7833/35.5311</f>
+        <v>0.89452057493294601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -518,8 +563,16 @@
         <f t="shared" si="0"/>
         <v>23.240159999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f>51.591/56.6322</f>
+        <v>0.910983504084249</v>
+      </c>
+      <c r="F7">
+        <f>51.5901/56.6322</f>
+        <v>0.91096761206522092</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -533,8 +586,16 @@
         <f t="shared" si="0"/>
         <v>17.095679999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f>38.552/45.678</f>
+        <v>0.8439949209685188</v>
+      </c>
+      <c r="F8">
+        <f>38.552/45.678</f>
+        <v>0.8439949209685188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -548,8 +609,16 @@
         <f t="shared" si="0"/>
         <v>17.029792</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>38.6/41.1682</f>
+        <v>0.93761689847989471</v>
+      </c>
+      <c r="F9">
+        <f>38.6/41.16822</f>
+        <v>0.93761644297470237</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -563,8 +632,16 @@
         <f t="shared" si="0"/>
         <v>14.769888000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f>34.4685/37.0638</f>
+        <v>0.92997749825975751</v>
+      </c>
+      <c r="F10">
+        <f>34.468572/37.063807</f>
+        <v>0.92997926521687324</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -578,8 +655,16 @@
         <f t="shared" si="0"/>
         <v>11.650864</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f>28.6625/29.4184</f>
+        <v>0.97430519674761384</v>
+      </c>
+      <c r="F11">
+        <f>28.6625/29.4184</f>
+        <v>0.97430519674761384</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -593,8 +678,16 @@
         <f t="shared" si="0"/>
         <v>7.2919840000000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f>16.5524/16.7974</f>
+        <v>0.98541440937287905</v>
+      </c>
+      <c r="F12">
+        <f>16.5524/16.7974</f>
+        <v>0.98541440937287905</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -608,8 +701,16 @@
         <f t="shared" si="0"/>
         <v>13.142975999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>29.2376/29.9596</f>
+        <v>0.97590087985153351</v>
+      </c>
+      <c r="F13">
+        <f>29.2376/29.9596</f>
+        <v>0.97590087985153351</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -623,8 +724,16 @@
         <f t="shared" si="0"/>
         <v>13.142975999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <f>30.5607/31.0304</f>
+        <v>0.98486323089615346</v>
+      </c>
+      <c r="F14">
+        <f>30.5607/31.0304</f>
+        <v>0.98486323089615346</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -637,6 +746,14 @@
       <c r="D15">
         <f t="shared" si="0"/>
         <v>14.081760000000001</v>
+      </c>
+      <c r="E15">
+        <f>31.4635/34.6892</f>
+        <v>0.90701140412577974</v>
+      </c>
+      <c r="F15">
+        <f>31.46358/34.6892</f>
+        <v>0.90701371031906186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Attempt VII - Created two more config files. a) for flowcapacity = 0.05 and beam.agentsim.agents.modalBehaviors.transitVehicleTypeVOTMultipliers = 2.0 b) for flowcapacity = 0.045 and beam.agentsim.agents.modalBehaviors.transitVehicleTypeVOTMultipliers = 2.0 + beam.physsim.network.overwriteRoadTypeProperties set to 10% lower than those set for 0.06
</commit_message>
<xml_diff>
--- a/SpeedCalculations.xlsx
+++ b/SpeedCalculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LBNL\LBNL-BEAM\beam-data-austin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E082A44-593F-4837-89C4-61F3893E60AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FBEAAA-29E0-4ADD-A291-331D70240266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27240" yWindow="1200" windowWidth="13605" windowHeight="14985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -408,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -423,7 +423,7 @@
     <col min="5" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -436,8 +436,11 @@
       <c r="F1">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -479,8 +482,16 @@
         <f>56.5051/67.3424</f>
         <v>0.83907166955736656</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <f>B3*E3*$G$1</f>
+        <v>23.631211747012284</v>
+      </c>
+      <c r="H3">
+        <f>G3/B3</f>
+        <v>0.75516450260162993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -502,8 +513,16 @@
         <f>51.6663/64.7336</f>
         <v>0.79813728882682256</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <f t="shared" ref="G4:G15" si="1">B4*E4*$G$1</f>
+        <v>20.872758675432852</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H15" si="2">G4/B4</f>
+        <v>0.71832355994414032</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -525,8 +544,16 @@
         <f>42.9408/47.1749</f>
         <v>0.91024676257925297</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>17.492029987132987</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="2"/>
+        <v>0.81922208632132765</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -548,8 +575,16 @@
         <f>31.7833/35.5311</f>
         <v>0.89452057493294601</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>12.785776166569569</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="2"/>
+        <v>0.80506851743965147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -571,8 +606,16 @@
         <f>51.5901/56.6322</f>
         <v>0.91096761206522092</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>21.171402392278598</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="2"/>
+        <v>0.81988515367582404</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -594,8 +637,16 @@
         <f>38.552/45.678</f>
         <v>0.8439949209685188</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>15.459286168396167</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="2"/>
+        <v>0.75959542887166698</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -617,8 +668,16 @@
         <f>38.6/41.16822</f>
         <v>0.93761644297470237</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>15.287956043742504</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="2"/>
+        <v>0.84385520863190533</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -640,8 +699,16 @@
         <f>34.468572/37.063807</f>
         <v>0.92997926521687324</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>13.29257757272595</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>0.83697974843378187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -663,8 +730,16 @@
         <f>28.6625/29.4184</f>
         <v>0.97430519674761384</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>10.532317121257446</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
+        <v>0.87687467707285249</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -686,8 +761,16 @@
         <f>16.5524/16.7974</f>
         <v>0.98541440937287905</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>6.5990443835355475</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="2"/>
+        <v>0.88687296843559127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -709,8 +792,16 @@
         <f>29.2376/29.9596</f>
         <v>0.97590087985153351</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>11.779201691878397</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>0.87831079186638017</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -732,8 +823,16 @@
         <f>30.5607/31.0304</f>
         <v>0.98486323089615346</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>11.887377985975043</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>0.88637690780653811</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -754,6 +853,14 @@
       <c r="F15">
         <f>31.46358/34.6892</f>
         <v>0.90701371031906186</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>12.772316910162241</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0.81631026371320181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>